<commit_message>
mise à jour mobile
</commit_message>
<xml_diff>
--- a/xlsform_template_survey.xlsx
+++ b/xlsform_template_survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helpdesk\OneDrive - AITS\Bureau\MASTER IA DATA SCIENCE DIT\RECHERCHES\MS Paiement digital RDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DBA649-DCDE-4706-93C7-ADF702B8C971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A1F4FB-63EA-4B73-8796-0D3A4A2AE78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2C89006E-A6DA-4E76-9E38-62F04CB62B10}"/>
   </bookViews>
@@ -1541,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8C8BA1-3870-495E-BE82-94E8BB581ACE}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,6 +1554,7 @@
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="53.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2263,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E7A6B2-212E-4B1B-9036-550D8D0084B9}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="83" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>